<commit_message>
Working on calculating useful energy
</commit_message>
<xml_diff>
--- a/inst/extdata/hmw_analysis_data.xlsx
+++ b/inst/extdata/hmw_analysis_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="825" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="825"/>
   </bookViews>
   <sheets>
     <sheet name="hmw_food" sheetId="1" r:id="rId1"/>
@@ -353,9 +353,6 @@
     <t>HMW.Region.code</t>
   </si>
   <si>
-    <t>kcal/day</t>
-  </si>
-  <si>
     <t>W</t>
   </si>
   <si>
@@ -387,6 +384,9 @@
   </si>
   <si>
     <t>Unit</t>
+  </si>
+  <si>
+    <t>kcal/day per person</t>
   </si>
 </sst>
 </file>
@@ -21638,8 +21638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM57"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21647,7 +21647,7 @@
     <col min="1" max="1" width="10.140625" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="15" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="9.140625" style="35"/>
     <col min="62" max="64" width="9.140625" style="11"/>
   </cols>
@@ -21663,7 +21663,7 @@
         <v>68</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E1" s="29">
         <v>1960</v>
@@ -21860,7 +21860,7 @@
         <v>19</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E2" s="31">
         <f t="array" ref="E2:BH8">TRANSPOSE('PS Data - Food Consumption'!C12:I67)</f>
@@ -22063,7 +22063,7 @@
         <v>21</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E3" s="31">
         <v>2232.6342117058821</v>
@@ -22265,7 +22265,7 @@
         <v>23</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E4" s="31">
         <v>2314.9779005121395</v>
@@ -22467,7 +22467,7 @@
         <v>25</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E5" s="31">
         <v>2163.5854668235302</v>
@@ -22669,7 +22669,7 @@
         <v>27</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E6" s="31">
         <v>2098.9607933000002</v>
@@ -22871,7 +22871,7 @@
         <v>29</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E7" s="31">
         <v>2173.3073561230763</v>
@@ -23073,7 +23073,7 @@
         <v>31</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E8" s="31">
         <v>2171.8971961223774</v>
@@ -23275,7 +23275,7 @@
         <v>19</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E9" s="31">
         <f t="array" ref="E9:BH15">TRANSPOSE('PS Data - Food Consumption'!U12:AA67)</f>
@@ -23478,7 +23478,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E10" s="31">
         <v>3348.9513175588236</v>
@@ -23680,7 +23680,7 @@
         <v>23</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E11" s="31">
         <v>3472.4668507682095</v>
@@ -23882,7 +23882,7 @@
         <v>25</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E12" s="31">
         <v>3245.3782002352955</v>
@@ -24084,7 +24084,7 @@
         <v>27</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E13" s="31">
         <v>3148.4411899500005</v>
@@ -24286,7 +24286,7 @@
         <v>29</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E14" s="31">
         <v>3259.9610341846151</v>
@@ -24488,7 +24488,7 @@
         <v>31</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E15" s="31">
         <v>3257.8457941835663</v>
@@ -24690,7 +24690,7 @@
         <v>19</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E16" s="31">
         <f t="array" ref="E16:BH22">TRANSPOSE('PS Data - Food Consumption'!AM12:AS67)</f>
@@ -24893,7 +24893,7 @@
         <v>21</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E17" s="31">
         <v>2870.5297007647059</v>
@@ -25095,7 +25095,7 @@
         <v>23</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E18" s="31">
         <v>2976.4001578013226</v>
@@ -25297,7 +25297,7 @@
         <v>25</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E19" s="31">
         <v>2781.7527430588243</v>
@@ -25499,7 +25499,7 @@
         <v>27</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E20" s="31">
         <v>2698.6638771000003</v>
@@ -25701,7 +25701,7 @@
         <v>29</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E21" s="31">
         <v>2794.2523150153843</v>
@@ -25903,7 +25903,7 @@
         <v>31</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E22" s="31">
         <v>2792.4392521573427</v>
@@ -26105,7 +26105,7 @@
         <v>19</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E23" s="31">
         <f t="array" ref="E23:BH29">TRANSPOSE('PS Data - Food Consumption'!L12:R67)</f>
@@ -26308,7 +26308,7 @@
         <v>21</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E24" s="31">
         <v>1924.7377956470584</v>
@@ -26510,7 +26510,7 @@
         <v>23</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E25" s="31">
         <v>2005.7744417738511</v>
@@ -26712,7 +26712,7 @@
         <v>25</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E26" s="31">
         <v>1856.7850625882359</v>
@@ -26914,7 +26914,7 @@
         <v>27</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E27" s="31">
         <v>1793.1861775333334</v>
@@ -27116,7 +27116,7 @@
         <v>29</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E28" s="31">
         <v>1866.352636184615</v>
@@ -27318,7 +27318,7 @@
         <v>31</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E29" s="31">
         <v>1864.9648596759907</v>
@@ -27520,7 +27520,7 @@
         <v>19</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E30" s="31">
         <f t="array" ref="E30:BH36">TRANSPOSE('PS Data - Food Consumption'!AD12:AJ67)</f>
@@ -27723,7 +27723,7 @@
         <v>21</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E31" s="32">
         <v>2749.6254223529409</v>
@@ -27925,7 +27925,7 @@
         <v>23</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E32" s="32">
         <v>2865.3920596769303</v>
@@ -28127,7 +28127,7 @@
         <v>25</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E33" s="32">
         <v>2652.5500894117658</v>
@@ -28329,7 +28329,7 @@
         <v>27</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E34" s="32">
         <v>2561.6945393333335</v>
@@ -28531,7 +28531,7 @@
         <v>29</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E35" s="32">
         <v>2666.2180516923072</v>
@@ -28733,7 +28733,7 @@
         <v>31</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E36" s="32">
         <v>2664.235513822844</v>
@@ -28935,7 +28935,7 @@
         <v>19</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E37" s="32">
         <f t="array" ref="E37:BH43">TRANSPOSE('PS Data - Food Consumption'!AV12:BB67)</f>
@@ -29138,7 +29138,7 @@
         <v>21</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E38" s="32">
         <v>2337.1816089999998</v>
@@ -29340,7 +29340,7 @@
         <v>23</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E39" s="32">
         <v>2435.5832507253908</v>
@@ -29542,7 +29542,7 @@
         <v>25</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E40" s="32">
         <v>2254.6675760000007</v>
@@ -29744,7 +29744,7 @@
         <v>27</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E41" s="32">
         <v>2177.4403584333336</v>
@@ -29946,7 +29946,7 @@
         <v>29</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E42" s="32">
         <v>2266.2853439384612</v>
@@ -30148,7 +30148,7 @@
         <v>31</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E43" s="32">
         <v>2264.6001867494174</v>
@@ -30432,15 +30432,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>64</v>
@@ -30448,7 +30448,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>65</v>
@@ -30456,7 +30456,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>67</v>
@@ -30464,26 +30464,26 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="15" t="s">
         <v>78</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -30495,7 +30495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="4" topLeftCell="AJ1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="D2" sqref="D2"/>
     </sheetView>
@@ -30522,7 +30522,7 @@
         <v>68</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E1" s="29">
         <v>1960</v>
@@ -30719,7 +30719,7 @@
         <v>19</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E2" s="31">
         <f t="array" ref="E2:BH2">TRANSPOSE('PS Data - Human Power Outputs'!C5:C60)</f>
@@ -30922,7 +30922,7 @@
         <v>21</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E3" s="31">
         <f t="array" ref="E3:BH3">TRANSPOSE('PS Data - Human Power Outputs'!E5:E60)</f>
@@ -31125,7 +31125,7 @@
         <v>23</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E4" s="31">
         <f t="array" ref="E4:BH4">TRANSPOSE('PS Data - Human Power Outputs'!G5:G60)</f>
@@ -31328,7 +31328,7 @@
         <v>25</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E5" s="31">
         <f t="array" ref="E5:BH5">TRANSPOSE('PS Data - Human Power Outputs'!I5:I60)</f>
@@ -31531,7 +31531,7 @@
         <v>27</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E6" s="31">
         <f t="array" ref="E6:BH6">TRANSPOSE('PS Data - Human Power Outputs'!K5:K60)</f>
@@ -31734,7 +31734,7 @@
         <v>29</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E7" s="31">
         <f t="array" ref="E7:BH7">TRANSPOSE('PS Data - Human Power Outputs'!M5:M60)</f>
@@ -31937,7 +31937,7 @@
         <v>31</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E8" s="31">
         <f t="array" ref="E8:BH8">TRANSPOSE('PS Data - Human Power Outputs'!O5:O60)</f>
@@ -32140,7 +32140,7 @@
         <v>19</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E9" s="31">
         <f t="array" ref="E9:BH9">TRANSPOSE('PS Data - Human Power Outputs'!D5:D60)</f>
@@ -32343,7 +32343,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E10" s="31">
         <f t="array" ref="E10:BH10">TRANSPOSE('PS Data - Human Power Outputs'!F5:F60)</f>
@@ -32546,7 +32546,7 @@
         <v>23</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E11" s="31">
         <f t="array" ref="E11:BH11">TRANSPOSE('PS Data - Human Power Outputs'!H5:H60)</f>
@@ -32749,7 +32749,7 @@
         <v>25</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E12" s="31">
         <f t="array" ref="E12:BH12">TRANSPOSE('PS Data - Human Power Outputs'!J5:J60)</f>
@@ -32952,7 +32952,7 @@
         <v>27</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E13" s="31">
         <f t="array" ref="E13:BH13">TRANSPOSE('PS Data - Human Power Outputs'!L5:L60)</f>
@@ -33155,7 +33155,7 @@
         <v>29</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E14" s="31">
         <f t="array" ref="E14:BH14">TRANSPOSE('PS Data - Human Power Outputs'!N5:N60)</f>
@@ -33358,7 +33358,7 @@
         <v>31</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E15" s="31">
         <f t="array" ref="E15:BH15">TRANSPOSE('PS Data - Human Power Outputs'!P5:P60)</f>
@@ -33561,7 +33561,7 @@
         <v>19</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E16" s="31">
         <f t="array" ref="E16:BH16">TRANSPOSE('PS Data - Human Power Outputs'!S5:S60)</f>
@@ -33764,7 +33764,7 @@
         <v>21</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E17" s="31">
         <f t="array" ref="E17:BH17">TRANSPOSE('PS Data - Human Power Outputs'!U5:U60)</f>
@@ -33967,7 +33967,7 @@
         <v>23</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E18" s="31">
         <f t="array" ref="E18:BH18">TRANSPOSE('PS Data - Human Power Outputs'!W5:W60)</f>
@@ -34170,7 +34170,7 @@
         <v>25</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E19" s="31">
         <f t="array" ref="E19:BH19">TRANSPOSE('PS Data - Human Power Outputs'!Y5:Y60)</f>
@@ -34373,7 +34373,7 @@
         <v>27</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E20" s="31">
         <f t="array" ref="E20:BH20">TRANSPOSE('PS Data - Human Power Outputs'!AA5:AA60)</f>
@@ -34576,7 +34576,7 @@
         <v>29</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E21" s="31">
         <f t="array" ref="E21:BH21">TRANSPOSE('PS Data - Human Power Outputs'!AC5:AC60)</f>
@@ -34779,7 +34779,7 @@
         <v>31</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E22" s="31">
         <f t="array" ref="E22:BH22">TRANSPOSE('PS Data - Human Power Outputs'!AE5:AE60)</f>
@@ -34982,7 +34982,7 @@
         <v>19</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E23" s="31">
         <f t="array" ref="E23:BH23">TRANSPOSE('PS Data - Human Power Outputs'!T5:T60)</f>
@@ -35185,7 +35185,7 @@
         <v>21</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E24" s="31">
         <f t="array" ref="E24:BH24">TRANSPOSE('PS Data - Human Power Outputs'!V5:V60)</f>
@@ -35388,7 +35388,7 @@
         <v>23</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E25" s="31">
         <f t="array" ref="E25:BH25">TRANSPOSE('PS Data - Human Power Outputs'!X5:X60)</f>
@@ -35591,7 +35591,7 @@
         <v>25</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E26" s="31">
         <f t="array" ref="E26:BH26">TRANSPOSE('PS Data - Human Power Outputs'!Z5:Z60)</f>
@@ -35794,7 +35794,7 @@
         <v>27</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E27" s="31">
         <f t="array" ref="E27:BH27">TRANSPOSE('PS Data - Human Power Outputs'!AB5:AB60)</f>
@@ -35997,7 +35997,7 @@
         <v>29</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E28" s="31">
         <f t="array" ref="E28:BH28">TRANSPOSE('PS Data - Human Power Outputs'!AD5:AD60)</f>
@@ -36200,7 +36200,7 @@
         <v>31</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E29" s="31">
         <f t="array" ref="E29:BH29">TRANSPOSE('PS Data - Human Power Outputs'!AF5:AF60)</f>

</xml_diff>